<commit_message>
update multi-scenario MORDM, domain criterion completed
</commit_message>
<xml_diff>
--- a/final assignment/results/selected_ref_scenarios.xlsx
+++ b/final assignment/results/selected_ref_scenarios.xlsx
@@ -428,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -681,125 +681,63 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1">
-        <v>699</v>
+        <v>853</v>
       </c>
       <c r="B5">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="C5">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="D5">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="E5">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="F5">
-        <v>210.837332337471</v>
+        <v>160.0267073656128</v>
       </c>
       <c r="G5">
-        <v>0.1233872329405957</v>
+        <v>0.3948806410290039</v>
       </c>
       <c r="H5">
+        <v>1.5</v>
+      </c>
+      <c r="I5">
+        <v>70.50616791972016</v>
+      </c>
+      <c r="J5">
+        <v>0.03704534369103996</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>284.8317160212392</v>
+      </c>
+      <c r="M5">
+        <v>0.00380201351087276</v>
+      </c>
+      <c r="N5">
         <v>10</v>
       </c>
-      <c r="I5">
-        <v>183.036688532314</v>
-      </c>
-      <c r="J5">
-        <v>0.07378790919099233</v>
-      </c>
-      <c r="K5">
-        <v>1.5</v>
-      </c>
-      <c r="L5">
-        <v>138.9027666952728</v>
-      </c>
-      <c r="M5">
-        <v>0.04556433583350048</v>
-      </c>
-      <c r="N5">
-        <v>1.5</v>
-      </c>
       <c r="O5">
-        <v>180.8170079028244</v>
+        <v>223.1764298548397</v>
       </c>
       <c r="P5">
-        <v>0.6595289098356109</v>
+        <v>0.9299987522121724</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="R5">
-        <v>212.7990361039125</v>
+        <v>289.4478818508682</v>
       </c>
       <c r="S5">
-        <v>0.8522874495026292</v>
+        <v>0.3993819532902357</v>
       </c>
       <c r="T5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="1">
-        <v>853</v>
-      </c>
-      <c r="B6">
-        <v>4.5</v>
-      </c>
-      <c r="C6">
-        <v>4.5</v>
-      </c>
-      <c r="D6">
-        <v>3.5</v>
-      </c>
-      <c r="E6">
-        <v>75</v>
-      </c>
-      <c r="F6">
-        <v>160.0267073656128</v>
-      </c>
-      <c r="G6">
-        <v>0.3948806410290039</v>
-      </c>
-      <c r="H6">
-        <v>1.5</v>
-      </c>
-      <c r="I6">
-        <v>70.50616791972016</v>
-      </c>
-      <c r="J6">
-        <v>0.03704534369103996</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>284.8317160212392</v>
-      </c>
-      <c r="M6">
-        <v>0.00380201351087276</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>223.1764298548397</v>
-      </c>
-      <c r="P6">
-        <v>0.9299987522121724</v>
-      </c>
-      <c r="Q6">
-        <v>1.5</v>
-      </c>
-      <c r="R6">
-        <v>289.4478818508682</v>
-      </c>
-      <c r="S6">
-        <v>0.3993819532902357</v>
-      </c>
-      <c r="T6">
         <v>1</v>
       </c>
     </row>

</xml_diff>